<commit_message>
Fixed reading of Expected Format
</commit_message>
<xml_diff>
--- a/Data/SABR  Plan Evaluation Worksheet BLANK May 2021 For Testing.xlsx
+++ b/Data/SABR  Plan Evaluation Worksheet BLANK May 2021 For Testing.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2499" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="627">
   <si>
     <t>Patient:</t>
   </si>
@@ -2855,6 +2855,9 @@
     <t>F8</t>
   </si>
   <si>
+    <t>F9</t>
+  </si>
+  <si>
     <t>G3</t>
   </si>
   <si>
@@ -2900,18 +2903,81 @@
     <t>StomachV1120</t>
   </si>
   <si>
+    <t>PTV Maximum Dose (%)</t>
+  </si>
+  <si>
+    <t>V 700 cGy</t>
+  </si>
+  <si>
+    <t>V 740 cGy</t>
+  </si>
+  <si>
+    <t>Aorta V31Gy</t>
+  </si>
+  <si>
+    <t>V 3100 cGy</t>
+  </si>
+  <si>
+    <t>Artery-Pulmonary V31Gy</t>
+  </si>
+  <si>
+    <t>V 1000 cGy</t>
+  </si>
+  <si>
+    <t>Ipsilat. Brach. Plex. V14Gy</t>
+  </si>
+  <si>
+    <t>V 1400 cGy</t>
+  </si>
+  <si>
+    <t>Skin V26Gy</t>
+  </si>
+  <si>
+    <t>V 2600 cGy</t>
+  </si>
+  <si>
+    <t>Skin V23Gy</t>
+  </si>
+  <si>
+    <t>V 2300 cGy</t>
+  </si>
+  <si>
+    <t>V 1190 cGy</t>
+  </si>
+  <si>
+    <t>Chestwall (rib) V22Gy</t>
+  </si>
+  <si>
+    <t>V 2200 cGy</t>
+  </si>
+  <si>
+    <t>V 1050 cGy</t>
+  </si>
+  <si>
+    <t>V 1120 cGy</t>
+  </si>
+  <si>
     <t>ProxTrachV1050</t>
   </si>
   <si>
     <t>ProxBronchV1050</t>
   </si>
   <si>
+    <t>F18</t>
+  </si>
+  <si>
     <t>F16</t>
   </si>
   <si>
     <t>F17</t>
   </si>
   <si>
+    <t>F20</t>
+  </si>
+  <si>
+    <t>F21</t>
+  </si>
+  <si>
     <t>F23</t>
   </si>
   <si>
@@ -2921,36 +2987,81 @@
     <t>F27</t>
   </si>
   <si>
+    <t>F28</t>
+  </si>
+  <si>
+    <t>F29</t>
+  </si>
+  <si>
     <t>F30</t>
   </si>
   <si>
+    <t>F31</t>
+  </si>
+  <si>
     <t>F32</t>
   </si>
   <si>
+    <t>F33</t>
+  </si>
+  <si>
     <t>F34</t>
   </si>
   <si>
+    <t>F35</t>
+  </si>
+  <si>
+    <t>F36</t>
+  </si>
+  <si>
+    <t>F37</t>
+  </si>
+  <si>
     <t>F38</t>
   </si>
   <si>
+    <t>F39</t>
+  </si>
+  <si>
+    <t>F40</t>
+  </si>
+  <si>
+    <t>F41</t>
+  </si>
+  <si>
     <t>F42</t>
   </si>
   <si>
     <t>F43</t>
   </si>
   <si>
+    <t>F44</t>
+  </si>
+  <si>
     <t>F45</t>
   </si>
   <si>
+    <t>F46</t>
+  </si>
+  <si>
     <t>F47</t>
   </si>
   <si>
     <t>F48</t>
   </si>
   <si>
+    <t>B49</t>
+  </si>
+  <si>
+    <t>C49</t>
+  </si>
+  <si>
     <t>F50</t>
   </si>
   <si>
+    <t>F51</t>
+  </si>
+  <si>
     <t>Address Check</t>
   </si>
   <si>
@@ -2972,18 +3083,6 @@
     <t>Constructor'</t>
   </si>
   <si>
-    <t>LungVolume</t>
-  </si>
-  <si>
-    <t>High_Dose_Spillage</t>
-  </si>
-  <si>
-    <t>0.000</t>
-  </si>
-  <si>
-    <t>High_Dose_SpillageVolume</t>
-  </si>
-  <si>
     <t>Aorta  (max point dose cGy)</t>
   </si>
   <si>
@@ -3051,6 +3150,24 @@
   </si>
   <si>
     <t>Stomach and Intestines V11.2Gy (cc) =</t>
+  </si>
+  <si>
+    <t>Spinal Canal V10Gy</t>
+  </si>
+  <si>
+    <t>Spinal Canal V7Gy</t>
+  </si>
+  <si>
+    <t>Esophagus V11.9Gy</t>
+  </si>
+  <si>
+    <t>Proximal Trachea V10.5Gy</t>
+  </si>
+  <si>
+    <t>Proximal Bronchial Tree V10.5Gy</t>
+  </si>
+  <si>
+    <t>Stomach and Intestines V11.2Gy</t>
   </si>
 </sst>
 </file>
@@ -4000,7 +4117,7 @@
     <xf numFmtId="0" fontId="34" fillId="9" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="50" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="400">
+  <cellXfs count="399">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4982,7 +5099,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -5022,24 +5138,6 @@
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="147">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -6139,6 +6237,24 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -7368,16 +7484,16 @@
     <tableColumn id="5" name="Address">
       <calculatedColumnFormula>SUBSTITUTE(Q4,"$","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Extracted Format" dataDxfId="2">
+    <tableColumn id="6" name="Extracted Format" dataDxfId="110">
       <calculatedColumnFormula>VLOOKUP(CELL("format",INDIRECT(Q4)),FormatLookup[],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Expected Format" dataDxfId="0">
+    <tableColumn id="7" name="Expected Format" dataDxfId="111">
       <calculatedColumnFormula>VLOOKUP(R4,Definitions34Gy1F[],3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Units" dataDxfId="1">
+    <tableColumn id="8" name="Units" dataDxfId="112">
       <calculatedColumnFormula>IF(ISBLANK(VLOOKUP(R4,Definitions34Gy1F[],5,FALSE)),"",VLOOKUP(R4,Definitions34Gy1F[],5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Address Check" dataDxfId="3">
+    <tableColumn id="9" name="Address Check" dataDxfId="113">
       <calculatedColumnFormula>EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" name="Format Check" dataDxfId="117">
@@ -7392,13 +7508,13 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Definitions34Gy1F" displayName="Definitions34Gy1F" ref="AA3:AJ48" totalsRowShown="0">
-  <autoFilter ref="AA3:AJ48"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Definitions34Gy1F" displayName="Definitions34Gy1F" ref="AA3:AJ47" totalsRowShown="0">
+  <autoFilter ref="AA3:AJ47"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Address"/>
-    <tableColumn id="3" name="Format" dataDxfId="5"/>
-    <tableColumn id="4" name="Extracted Format" dataDxfId="4"/>
+    <tableColumn id="3" name="Format" dataDxfId="115"/>
+    <tableColumn id="4" name="Extracted Format" dataDxfId="114"/>
     <tableColumn id="5" name="Units"/>
     <tableColumn id="6" name="Label"/>
     <tableColumn id="7" name="Reference"/>
@@ -12173,69 +12289,69 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K30:K52">
-    <cfRule type="containsText" dxfId="115" priority="17" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="109" priority="17" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:K14 K21:K29 K19">
-    <cfRule type="containsText" dxfId="114" priority="14" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="108" priority="14" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="15" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="107" priority="15" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="16" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="106" priority="16" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="111" priority="12" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="105" priority="12" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="13" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="104" priority="13" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="containsText" dxfId="109" priority="11" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="103" priority="11" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="108" priority="10" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="102" priority="10" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="containsText" dxfId="107" priority="7" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="101" priority="7" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="8" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="100" priority="8" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="9" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="99" priority="9" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="104" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="98" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="5" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="97" priority="5" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="6" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="96" priority="6" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="101" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="95" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="2" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="94" priority="2" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="3" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="93" priority="3" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16239,80 +16355,80 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K28:K44">
-    <cfRule type="containsText" dxfId="98" priority="22" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="92" priority="22" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:K26">
-    <cfRule type="containsText" dxfId="97" priority="20" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="91" priority="20" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K19)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="21" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="90" priority="21" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:K24">
-    <cfRule type="containsText" dxfId="95" priority="17" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="89" priority="17" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27">
-    <cfRule type="containsText" dxfId="94" priority="11" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="88" priority="11" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="12" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="87" priority="12" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="16" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="86" priority="16" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:K14">
-    <cfRule type="containsText" dxfId="91" priority="13" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="85" priority="13" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="14" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="84" priority="14" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="15" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="83" priority="15" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="88" priority="10" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="82" priority="10" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="containsText" dxfId="87" priority="7" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="81" priority="7" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="8" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="80" priority="8" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="9" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="79" priority="9" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="84" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="78" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="5" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="77" priority="5" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="6" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="76" priority="6" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="81" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="75" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="2" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="74" priority="2" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="3" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="73" priority="3" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17393,136 +17509,136 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K14 K35 K39:K40 K19:K27">
-    <cfRule type="containsText" dxfId="78" priority="41" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="72" priority="41" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="77" priority="40" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="71" priority="40" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="76" priority="39" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="70" priority="39" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="75" priority="38" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="69" priority="38" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33">
-    <cfRule type="containsText" dxfId="74" priority="37" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="68" priority="37" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="containsText" dxfId="73" priority="36" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="67" priority="36" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36">
-    <cfRule type="containsText" dxfId="72" priority="35" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="66" priority="35" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37">
-    <cfRule type="containsText" dxfId="71" priority="34" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="65" priority="34" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38">
-    <cfRule type="containsText" dxfId="70" priority="33" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="64" priority="33" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41">
-    <cfRule type="containsText" dxfId="69" priority="32" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="63" priority="32" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="68" priority="29" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="62" priority="29" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="30" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="61" priority="30" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="31" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="60" priority="31" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="containsText" dxfId="65" priority="16" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="59" priority="16" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="17" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="58" priority="17" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="18" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="57" priority="18" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="containsText" dxfId="62" priority="13" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="56" priority="13" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="14" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="55" priority="14" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="15" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="54" priority="15" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:K27">
-    <cfRule type="containsText" dxfId="59" priority="12" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="53" priority="12" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="19" stopIfTrue="1" operator="containsText" text="MAJOR">
+    <cfRule type="containsText" dxfId="52" priority="19" stopIfTrue="1" operator="containsText" text="MAJOR">
       <formula>NOT(ISERROR(SEARCH("MAJOR",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="containsText" dxfId="57" priority="11" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="51" priority="11" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="containsText" dxfId="56" priority="10" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="50" priority="10" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="containsText" dxfId="55" priority="7" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="49" priority="7" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="8" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="48" priority="8" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="9" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="47" priority="9" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="52" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="46" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="5" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="45" priority="5" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="6" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="44" priority="6" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="49" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="43" priority="1" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="2" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="42" priority="2" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="3" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="41" priority="3" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17539,13 +17655,13 @@
   </sheetPr>
   <dimension ref="A1:AJ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AG55" sqref="AG55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="3.85546875" customWidth="1"/>
@@ -17558,10 +17674,10 @@
     <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="2" customWidth="1"/>
     <col min="13" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="38.85546875" style="342" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.28515625" style="337" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="6.28515625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="23.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="43" style="342" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" style="337" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -17569,13 +17685,13 @@
     <col min="23" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="14" bestFit="1" customWidth="1"/>
@@ -17618,7 +17734,7 @@
         <v>117</v>
       </c>
       <c r="F3" s="81"/>
-      <c r="G3" s="394"/>
+      <c r="G3" s="393"/>
       <c r="H3" s="80"/>
       <c r="I3" s="80"/>
       <c r="J3" s="82" t="s">
@@ -17646,19 +17762,19 @@
         <v>372</v>
       </c>
       <c r="U3" s="388" t="s">
-        <v>557</v>
+        <v>594</v>
       </c>
       <c r="V3" s="373" t="s">
         <v>184</v>
       </c>
       <c r="W3" s="373" t="s">
-        <v>554</v>
+        <v>591</v>
       </c>
       <c r="X3" s="388" t="s">
-        <v>558</v>
+        <v>595</v>
       </c>
       <c r="Y3" s="373" t="s">
-        <v>559</v>
+        <v>596</v>
       </c>
       <c r="AA3" t="s">
         <v>181</v>
@@ -17688,7 +17804,7 @@
         <v>374</v>
       </c>
       <c r="AJ3" t="s">
-        <v>560</v>
+        <v>597</v>
       </c>
     </row>
     <row r="4" spans="2:36" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -17733,7 +17849,7 @@
         <v>General</v>
       </c>
       <c r="U4" s="347" t="s">
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="V4" s="348" t="str">
         <f>IF(ISBLANK(VLOOKUP(R4,Definitions34Gy1F[],5,FALSE)),"",VLOOKUP(R4,Definitions34Gy1F[],5,FALSE))</f>
@@ -17758,10 +17874,10 @@
         <v>515</v>
       </c>
       <c r="AC4" s="347" t="s">
-        <v>186</v>
+        <v>592</v>
       </c>
       <c r="AD4" s="347" t="s">
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="AF4" t="s">
         <v>0</v>
@@ -17837,10 +17953,10 @@
         <v>516</v>
       </c>
       <c r="AC5" s="347" t="s">
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="AD5" s="347" t="s">
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="AF5" t="s">
         <v>187</v>
@@ -17919,10 +18035,10 @@
         <v>517</v>
       </c>
       <c r="AC6" s="347" t="s">
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="AD6" s="347" t="s">
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="AF6" t="s">
         <v>2</v>
@@ -17999,10 +18115,10 @@
         <v>518</v>
       </c>
       <c r="AC7" s="347" t="s">
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="AD7" s="347" t="s">
-        <v>555</v>
+        <v>592</v>
       </c>
       <c r="AF7" t="s">
         <v>3</v>
@@ -18081,7 +18197,7 @@
         <v>431</v>
       </c>
       <c r="AD8" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE8" t="s">
         <v>194</v>
@@ -18156,7 +18272,7 @@
         <f>IF(ISERROR(FIND(config34Gy1F[[#This Row],[Units]],config34Gy1F[[#This Row],[Label]])),"Check",TRUE)</f>
         <v>1</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA9" s="4" t="s">
         <v>195</v>
       </c>
       <c r="AB9" t="s">
@@ -18166,7 +18282,7 @@
         <v>431</v>
       </c>
       <c r="AD9" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE9" t="s">
         <v>194</v>
@@ -18224,7 +18340,7 @@
         <f t="shared" ca="1" si="1"/>
         <v>F6</v>
       </c>
-      <c r="T10" s="390" t="str">
+      <c r="T10" s="347" t="str">
         <f ca="1">VLOOKUP(CELL("format",INDIRECT(Q10)),FormatLookup[],2,FALSE)</f>
         <v>0.00</v>
       </c>
@@ -18258,7 +18374,7 @@
         <v>431</v>
       </c>
       <c r="AD10" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE10" t="s">
         <v>194</v>
@@ -18344,16 +18460,16 @@
         <v>1</v>
       </c>
       <c r="AA11" t="s">
-        <v>561</v>
+        <v>197</v>
       </c>
       <c r="AB11" t="s">
-        <v>299</v>
+        <v>522</v>
       </c>
       <c r="AC11" s="347" t="s">
         <v>431</v>
       </c>
       <c r="AD11" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE11" t="s">
         <v>194</v>
@@ -18437,13 +18553,13 @@
         <v>190</v>
       </c>
       <c r="AB12" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AC12" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AD12" s="347" t="s">
-        <v>186</v>
+        <v>593</v>
       </c>
       <c r="AE12" t="s">
         <v>191</v>
@@ -18496,7 +18612,7 @@
         <f ca="1">CELL("address",F9)</f>
         <v>$F$9</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="4" t="s">
         <v>197</v>
       </c>
       <c r="S13" t="str">
@@ -18513,9 +18629,9 @@
       <c r="V13" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W13" t="e">
+      <c r="W13" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X13" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -18529,13 +18645,13 @@
         <v>192</v>
       </c>
       <c r="AB13" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="AC13" s="347" t="s">
-        <v>556</v>
+        <v>593</v>
       </c>
       <c r="AD13" s="347" t="s">
-        <v>186</v>
+        <v>593</v>
       </c>
       <c r="AF13" t="s">
         <v>116</v>
@@ -18603,7 +18719,7 @@
         <v>198</v>
       </c>
       <c r="AB14" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="AC14" s="347" t="s">
         <v>469</v>
@@ -18679,22 +18795,22 @@
         <v>1</v>
       </c>
       <c r="AA15" t="s">
-        <v>304</v>
+        <v>201</v>
       </c>
       <c r="AB15" t="s">
-        <v>305</v>
+        <v>558</v>
       </c>
       <c r="AC15" s="347" t="s">
-        <v>438</v>
+        <v>469</v>
       </c>
       <c r="AD15" s="347" t="s">
-        <v>438</v>
+        <v>469</v>
       </c>
       <c r="AE15" t="s">
         <v>199</v>
       </c>
       <c r="AF15" t="s">
-        <v>481</v>
+        <v>538</v>
       </c>
       <c r="AG15" t="s">
         <v>297</v>
@@ -18703,7 +18819,7 @@
         <v>293</v>
       </c>
       <c r="AJ15" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="16" spans="2:36" x14ac:dyDescent="0.2">
@@ -18776,7 +18892,7 @@
         <v>203</v>
       </c>
       <c r="AB16" t="s">
-        <v>539</v>
+        <v>559</v>
       </c>
       <c r="AC16" s="347" t="s">
         <v>469</v>
@@ -18852,9 +18968,9 @@
       <c r="V17" s="348" t="s">
         <v>199</v>
       </c>
-      <c r="W17" t="e">
+      <c r="W17" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X17" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -18868,7 +18984,7 @@
         <v>205</v>
       </c>
       <c r="AB17" t="s">
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="AC17" s="347" t="s">
         <v>469</v>
@@ -18945,9 +19061,9 @@
       <c r="V18" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W18" t="e">
+      <c r="W18" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X18" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -18958,16 +19074,16 @@
         <v>1</v>
       </c>
       <c r="AA18" t="s">
-        <v>562</v>
+        <v>207</v>
       </c>
       <c r="AB18" t="s">
-        <v>309</v>
+        <v>561</v>
       </c>
       <c r="AC18" s="347" t="s">
         <v>431</v>
       </c>
       <c r="AD18" s="347" t="s">
-        <v>563</v>
+        <v>431</v>
       </c>
       <c r="AE18" t="s">
         <v>194</v>
@@ -19028,9 +19144,9 @@
       <c r="V19" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W19" t="e">
+      <c r="W19" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X19" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -19041,16 +19157,16 @@
         <v>1</v>
       </c>
       <c r="AA19" t="s">
-        <v>564</v>
+        <v>209</v>
       </c>
       <c r="AB19" t="s">
-        <v>311</v>
+        <v>562</v>
       </c>
       <c r="AC19" s="347" t="s">
         <v>431</v>
       </c>
       <c r="AD19" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE19" t="s">
         <v>194</v>
@@ -19077,7 +19193,7 @@
       </c>
       <c r="D20" s="110"/>
       <c r="E20" s="112"/>
-      <c r="F20" s="391" t="s">
+      <c r="F20" s="390" t="s">
         <v>46</v>
       </c>
       <c r="G20" s="150" t="e">
@@ -19142,13 +19258,13 @@
         <v>211</v>
       </c>
       <c r="AB20" t="s">
-        <v>541</v>
+        <v>563</v>
       </c>
       <c r="AC20" s="347" t="s">
-        <v>514</v>
+        <v>469</v>
       </c>
       <c r="AD20" s="347" t="s">
-        <v>186</v>
+        <v>469</v>
       </c>
       <c r="AE20" t="s">
         <v>199</v>
@@ -19243,13 +19359,13 @@
         <v>213</v>
       </c>
       <c r="AB21" t="s">
-        <v>542</v>
+        <v>564</v>
       </c>
       <c r="AC21" s="347" t="s">
         <v>431</v>
       </c>
       <c r="AD21" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE21" t="s">
         <v>194</v>
@@ -19304,7 +19420,7 @@
         <f ca="1">VLOOKUP(CELL("format",INDIRECT(Q22)),FormatLookup[],2,FALSE)</f>
         <v>0.00%</v>
       </c>
-      <c r="U22" s="395" t="s">
+      <c r="U22" s="394" t="s">
         <v>438</v>
       </c>
       <c r="V22" s="348" t="str">
@@ -19324,22 +19440,22 @@
         <v>1</v>
       </c>
       <c r="AA22" t="s">
-        <v>316</v>
+        <v>215</v>
       </c>
       <c r="AB22" t="s">
-        <v>317</v>
+        <v>565</v>
       </c>
       <c r="AC22" s="347" t="s">
-        <v>514</v>
+        <v>438</v>
       </c>
       <c r="AD22" s="347" t="s">
         <v>438</v>
       </c>
       <c r="AE22" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="AF22" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="AG22" t="s">
         <v>141</v>
@@ -19348,10 +19464,10 @@
         <v>293</v>
       </c>
       <c r="AI22" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="AJ22" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:36" ht="14.25" x14ac:dyDescent="0.25">
@@ -19394,7 +19510,7 @@
         <v>$F$28</v>
       </c>
       <c r="R23" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="S23" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -19410,9 +19526,9 @@
       <c r="V23" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W23" t="e">
+      <c r="W23" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X23" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -19423,22 +19539,22 @@
         <v>Check</v>
       </c>
       <c r="AA23" t="s">
-        <v>318</v>
+        <v>526</v>
       </c>
       <c r="AB23" t="s">
-        <v>319</v>
+        <v>566</v>
       </c>
       <c r="AC23" s="347" t="s">
-        <v>514</v>
+        <v>431</v>
       </c>
       <c r="AD23" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE23" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AF23" t="s">
-        <v>389</v>
+        <v>44</v>
       </c>
       <c r="AG23" t="s">
         <v>141</v>
@@ -19450,7 +19566,7 @@
         <v>376</v>
       </c>
       <c r="AJ23" t="s">
-        <v>388</v>
+        <v>539</v>
       </c>
     </row>
     <row r="24" spans="1:36" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -19497,7 +19613,7 @@
         <v>$F$29</v>
       </c>
       <c r="R24" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -19513,9 +19629,9 @@
       <c r="V24" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W24" t="e">
+      <c r="W24" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X24" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -19526,22 +19642,22 @@
         <v>Check</v>
       </c>
       <c r="AA24" t="s">
-        <v>215</v>
+        <v>527</v>
       </c>
       <c r="AB24" t="s">
-        <v>543</v>
+        <v>567</v>
       </c>
       <c r="AC24" s="347" t="s">
-        <v>469</v>
+        <v>431</v>
       </c>
       <c r="AD24" s="347" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="AE24" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="AF24" t="s">
-        <v>390</v>
+        <v>45</v>
       </c>
       <c r="AG24" t="s">
         <v>141</v>
@@ -19553,7 +19669,7 @@
         <v>376</v>
       </c>
       <c r="AJ24" t="s">
-        <v>391</v>
+        <v>540</v>
       </c>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.2">
@@ -19578,7 +19694,7 @@
       <c r="L25" s="84"/>
       <c r="M25" s="85"/>
       <c r="O25" s="338" t="s">
-        <v>565</v>
+        <v>598</v>
       </c>
       <c r="P25" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -19623,13 +19739,13 @@
         <v>221</v>
       </c>
       <c r="AB25" t="s">
-        <v>544</v>
+        <v>568</v>
       </c>
       <c r="AC25" s="347" t="s">
         <v>514</v>
       </c>
       <c r="AD25" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AE25" t="s">
         <v>191</v>
@@ -19665,7 +19781,7 @@
       <c r="L26" s="84"/>
       <c r="M26" s="85"/>
       <c r="O26" s="338" t="s">
-        <v>576</v>
+        <v>609</v>
       </c>
       <c r="P26" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -19676,7 +19792,7 @@
         <v>$F$31</v>
       </c>
       <c r="R26" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="S26" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -19692,9 +19808,9 @@
       <c r="V26" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W26" t="e">
+      <c r="W26" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X26" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -19705,22 +19821,22 @@
         <v>1</v>
       </c>
       <c r="AA26" t="s">
-        <v>479</v>
+        <v>528</v>
       </c>
       <c r="AB26" t="s">
-        <v>485</v>
+        <v>569</v>
       </c>
       <c r="AC26" s="347" t="s">
         <v>431</v>
       </c>
       <c r="AD26" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE26" t="s">
         <v>194</v>
       </c>
       <c r="AF26" t="s">
-        <v>486</v>
+        <v>541</v>
       </c>
       <c r="AG26" t="s">
         <v>323</v>
@@ -19729,7 +19845,7 @@
         <v>293</v>
       </c>
       <c r="AJ26" t="s">
-        <v>480</v>
+        <v>542</v>
       </c>
     </row>
     <row r="27" spans="1:36" ht="14.25" x14ac:dyDescent="0.25">
@@ -19764,7 +19880,7 @@
       </c>
       <c r="M27" s="85"/>
       <c r="O27" s="338" t="s">
-        <v>566</v>
+        <v>599</v>
       </c>
       <c r="P27" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -19809,13 +19925,13 @@
         <v>225</v>
       </c>
       <c r="AB27" t="s">
-        <v>545</v>
+        <v>570</v>
       </c>
       <c r="AC27" s="347" t="s">
         <v>514</v>
       </c>
       <c r="AD27" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AE27" t="s">
         <v>191</v>
@@ -19845,7 +19961,7 @@
         <v>145</v>
       </c>
       <c r="E28" s="376"/>
-      <c r="F28" s="392" t="s">
+      <c r="F28" s="391" t="s">
         <v>46</v>
       </c>
       <c r="G28" s="188"/>
@@ -19864,7 +19980,7 @@
       <c r="M28" s="191"/>
       <c r="N28" s="4"/>
       <c r="O28" s="338" t="s">
-        <v>577</v>
+        <v>610</v>
       </c>
       <c r="P28" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -19875,7 +19991,7 @@
         <v>$F$33</v>
       </c>
       <c r="R28" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="S28" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -19891,9 +20007,9 @@
       <c r="V28" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W28" t="e">
+      <c r="W28" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X28" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -19904,22 +20020,22 @@
         <v>1</v>
       </c>
       <c r="AA28" t="s">
-        <v>487</v>
+        <v>529</v>
       </c>
       <c r="AB28" t="s">
-        <v>325</v>
+        <v>571</v>
       </c>
       <c r="AC28" s="347" t="s">
         <v>431</v>
       </c>
       <c r="AD28" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE28" t="s">
         <v>194</v>
       </c>
       <c r="AF28" t="s">
-        <v>488</v>
+        <v>543</v>
       </c>
       <c r="AG28" t="s">
         <v>326</v>
@@ -19928,7 +20044,7 @@
         <v>293</v>
       </c>
       <c r="AJ28" t="s">
-        <v>480</v>
+        <v>542</v>
       </c>
     </row>
     <row r="29" spans="1:36" ht="14.25" x14ac:dyDescent="0.25">
@@ -19962,7 +20078,7 @@
       <c r="M29" s="191"/>
       <c r="N29" s="4"/>
       <c r="O29" s="338" t="s">
-        <v>567</v>
+        <v>600</v>
       </c>
       <c r="P29" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20007,13 +20123,13 @@
         <v>229</v>
       </c>
       <c r="AB29" t="s">
-        <v>546</v>
+        <v>572</v>
       </c>
       <c r="AC29" s="347" t="s">
         <v>514</v>
       </c>
       <c r="AD29" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AE29" t="s">
         <v>191</v>
@@ -20063,7 +20179,7 @@
       </c>
       <c r="M30" s="85"/>
       <c r="O30" s="338" t="s">
-        <v>578</v>
+        <v>611</v>
       </c>
       <c r="P30" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20074,7 +20190,7 @@
         <v>$F$35</v>
       </c>
       <c r="R30" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="S30" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -20090,9 +20206,9 @@
       <c r="V30" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W30" t="e">
+      <c r="W30" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X30" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -20103,34 +20219,31 @@
         <v>1</v>
       </c>
       <c r="AA30" t="s">
-        <v>237</v>
+        <v>530</v>
       </c>
       <c r="AB30" t="s">
-        <v>547</v>
+        <v>573</v>
       </c>
       <c r="AC30" s="347" t="s">
-        <v>514</v>
+        <v>431</v>
       </c>
       <c r="AD30" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE30" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AF30" t="s">
-        <v>405</v>
+        <v>621</v>
       </c>
       <c r="AG30" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="AH30" t="s">
         <v>293</v>
       </c>
-      <c r="AI30" t="s">
-        <v>406</v>
-      </c>
       <c r="AJ30" t="s">
-        <v>384</v>
+        <v>544</v>
       </c>
     </row>
     <row r="31" spans="1:36" ht="14.25" x14ac:dyDescent="0.2">
@@ -20164,7 +20277,7 @@
       </c>
       <c r="M31" s="85"/>
       <c r="O31" s="338" t="s">
-        <v>579</v>
+        <v>612</v>
       </c>
       <c r="P31" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20175,7 +20288,7 @@
         <v>$F$36</v>
       </c>
       <c r="R31" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -20191,9 +20304,9 @@
       <c r="V31" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W31" t="e">
+      <c r="W31" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X31" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -20204,34 +20317,31 @@
         <v>1</v>
       </c>
       <c r="AA31" t="s">
-        <v>489</v>
+        <v>532</v>
       </c>
       <c r="AB31" t="s">
-        <v>329</v>
+        <v>574</v>
       </c>
       <c r="AC31" s="347" t="s">
         <v>431</v>
       </c>
       <c r="AD31" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE31" t="s">
         <v>194</v>
       </c>
       <c r="AF31" t="s">
-        <v>490</v>
+        <v>622</v>
       </c>
       <c r="AG31" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="AH31" t="s">
         <v>293</v>
       </c>
-      <c r="AI31" t="s">
-        <v>406</v>
-      </c>
       <c r="AJ31" t="s">
-        <v>410</v>
+        <v>539</v>
       </c>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.2">
@@ -20266,7 +20376,7 @@
       </c>
       <c r="M32" s="85"/>
       <c r="O32" s="338" t="s">
-        <v>568</v>
+        <v>601</v>
       </c>
       <c r="P32" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20293,9 +20403,9 @@
       <c r="V32" s="348" t="s">
         <v>191</v>
       </c>
-      <c r="W32" t="e">
+      <c r="W32" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X32" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -20306,25 +20416,25 @@
         <v>1</v>
       </c>
       <c r="AA32" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="AB32" t="s">
-        <v>548</v>
+        <v>575</v>
       </c>
       <c r="AC32" s="347" t="s">
         <v>514</v>
       </c>
       <c r="AD32" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AE32" t="s">
         <v>191</v>
       </c>
       <c r="AF32" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="AG32" t="s">
-        <v>16</v>
+        <v>332</v>
       </c>
       <c r="AH32" t="s">
         <v>293</v>
@@ -20362,7 +20472,7 @@
       </c>
       <c r="M33" s="85"/>
       <c r="O33" s="338" t="s">
-        <v>569</v>
+        <v>602</v>
       </c>
       <c r="P33" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20404,31 +20514,34 @@
         <v>1</v>
       </c>
       <c r="AA33" t="s">
-        <v>491</v>
+        <v>237</v>
       </c>
       <c r="AB33" t="s">
-        <v>331</v>
+        <v>576</v>
       </c>
       <c r="AC33" s="347" t="s">
-        <v>431</v>
+        <v>514</v>
       </c>
       <c r="AD33" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AE33" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AF33" t="s">
-        <v>492</v>
+        <v>405</v>
       </c>
       <c r="AG33" t="s">
-        <v>16</v>
+        <v>129</v>
       </c>
       <c r="AH33" t="s">
         <v>293</v>
       </c>
+      <c r="AI33" t="s">
+        <v>406</v>
+      </c>
       <c r="AJ33" t="s">
-        <v>480</v>
+        <v>384</v>
       </c>
     </row>
     <row r="34" spans="1:36" x14ac:dyDescent="0.2">
@@ -20463,7 +20576,7 @@
       </c>
       <c r="M34" s="85"/>
       <c r="O34" s="338" t="s">
-        <v>580</v>
+        <v>613</v>
       </c>
       <c r="P34" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20474,7 +20587,7 @@
         <v>$F$39</v>
       </c>
       <c r="R34" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="S34" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -20490,9 +20603,9 @@
       <c r="V34" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W34" t="e">
+      <c r="W34" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X34" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -20503,31 +20616,34 @@
         <v>1</v>
       </c>
       <c r="AA34" t="s">
-        <v>247</v>
+        <v>531</v>
       </c>
       <c r="AB34" t="s">
-        <v>549</v>
+        <v>577</v>
       </c>
       <c r="AC34" s="347" t="s">
-        <v>514</v>
+        <v>431</v>
       </c>
       <c r="AD34" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE34" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AF34" t="s">
-        <v>414</v>
+        <v>545</v>
       </c>
       <c r="AG34" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
       <c r="AH34" t="s">
         <v>293</v>
       </c>
+      <c r="AI34" t="s">
+        <v>406</v>
+      </c>
       <c r="AJ34" t="s">
-        <v>384</v>
+        <v>546</v>
       </c>
     </row>
     <row r="35" spans="1:36" ht="14.25" x14ac:dyDescent="0.25">
@@ -20559,7 +20675,7 @@
       </c>
       <c r="M35" s="85"/>
       <c r="O35" s="338" t="s">
-        <v>581</v>
+        <v>614</v>
       </c>
       <c r="P35" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20570,7 +20686,7 @@
         <v>$F$40</v>
       </c>
       <c r="R35" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="S35" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -20586,9 +20702,9 @@
       <c r="V35" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W35" t="e">
+      <c r="W35" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X35" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -20599,31 +20715,31 @@
         <v>1</v>
       </c>
       <c r="AA35" t="s">
-        <v>251</v>
+        <v>533</v>
       </c>
       <c r="AB35" t="s">
-        <v>550</v>
+        <v>578</v>
       </c>
       <c r="AC35" s="347" t="s">
-        <v>514</v>
+        <v>431</v>
       </c>
       <c r="AD35" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE35" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AF35" t="s">
-        <v>417</v>
+        <v>547</v>
       </c>
       <c r="AG35" t="s">
-        <v>341</v>
+        <v>14</v>
       </c>
       <c r="AH35" t="s">
         <v>293</v>
       </c>
       <c r="AJ35" t="s">
-        <v>384</v>
+        <v>548</v>
       </c>
     </row>
     <row r="36" spans="1:36" ht="14.25" x14ac:dyDescent="0.25">
@@ -20654,7 +20770,7 @@
       </c>
       <c r="M36" s="85"/>
       <c r="O36" s="338" t="s">
-        <v>582</v>
+        <v>615</v>
       </c>
       <c r="P36" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20665,7 +20781,7 @@
         <v>$F$41</v>
       </c>
       <c r="R36" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="S36" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -20681,9 +20797,9 @@
       <c r="V36" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W36" t="e">
+      <c r="W36" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X36" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -20694,31 +20810,31 @@
         <v>1</v>
       </c>
       <c r="AA36" t="s">
-        <v>493</v>
+        <v>534</v>
       </c>
       <c r="AB36" t="s">
-        <v>335</v>
+        <v>579</v>
       </c>
       <c r="AC36" s="347" t="s">
         <v>431</v>
       </c>
       <c r="AD36" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE36" t="s">
         <v>194</v>
       </c>
       <c r="AF36" t="s">
-        <v>494</v>
+        <v>549</v>
       </c>
       <c r="AG36" t="s">
-        <v>341</v>
+        <v>14</v>
       </c>
       <c r="AH36" t="s">
         <v>293</v>
       </c>
       <c r="AJ36" t="s">
-        <v>495</v>
+        <v>550</v>
       </c>
     </row>
     <row r="37" spans="1:36" x14ac:dyDescent="0.2">
@@ -20746,7 +20862,7 @@
       </c>
       <c r="M37" s="85"/>
       <c r="O37" s="338" t="s">
-        <v>570</v>
+        <v>603</v>
       </c>
       <c r="P37" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20788,25 +20904,25 @@
         <v>1</v>
       </c>
       <c r="AA37" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="AB37" t="s">
-        <v>551</v>
+        <v>580</v>
       </c>
       <c r="AC37" s="347" t="s">
         <v>514</v>
       </c>
       <c r="AD37" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AE37" t="s">
         <v>191</v>
       </c>
       <c r="AF37" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="AG37" t="s">
-        <v>136</v>
+        <v>16</v>
       </c>
       <c r="AH37" t="s">
         <v>293</v>
@@ -20845,7 +20961,7 @@
       </c>
       <c r="M38" s="85"/>
       <c r="O38" s="338" t="s">
-        <v>571</v>
+        <v>604</v>
       </c>
       <c r="P38" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20887,31 +21003,28 @@
         <v>1</v>
       </c>
       <c r="AA38" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="AB38" t="s">
-        <v>552</v>
+        <v>581</v>
       </c>
       <c r="AC38" s="347" t="s">
         <v>514</v>
       </c>
       <c r="AD38" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AE38" t="s">
         <v>191</v>
       </c>
       <c r="AF38" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="AG38" t="s">
-        <v>346</v>
+        <v>13</v>
       </c>
       <c r="AH38" t="s">
         <v>293</v>
-      </c>
-      <c r="AI38" t="s">
-        <v>406</v>
       </c>
       <c r="AJ38" t="s">
         <v>384</v>
@@ -20946,7 +21059,7 @@
       </c>
       <c r="M39" s="85"/>
       <c r="O39" s="338" t="s">
-        <v>583</v>
+        <v>616</v>
       </c>
       <c r="P39" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -20957,7 +21070,7 @@
         <v>$F$44</v>
       </c>
       <c r="R39" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="S39" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -20973,9 +21086,9 @@
       <c r="V39" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W39" t="e">
+      <c r="W39" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X39" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -20986,31 +21099,31 @@
         <v>1</v>
       </c>
       <c r="AA39" t="s">
-        <v>498</v>
+        <v>535</v>
       </c>
       <c r="AB39" t="s">
-        <v>499</v>
+        <v>582</v>
       </c>
       <c r="AC39" s="347" t="s">
         <v>431</v>
       </c>
       <c r="AD39" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE39" t="s">
         <v>194</v>
       </c>
       <c r="AF39" t="s">
-        <v>500</v>
+        <v>623</v>
       </c>
       <c r="AG39" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="AH39" t="s">
         <v>293</v>
       </c>
       <c r="AJ39" t="s">
-        <v>480</v>
+        <v>551</v>
       </c>
     </row>
     <row r="40" spans="1:36" ht="14.25" x14ac:dyDescent="0.25">
@@ -21025,7 +21138,7 @@
       <c r="E40" s="283" t="s">
         <v>169</v>
       </c>
-      <c r="F40" s="393" t="s">
+      <c r="F40" s="392" t="s">
         <v>46</v>
       </c>
       <c r="G40" s="219" t="s">
@@ -21045,7 +21158,7 @@
       </c>
       <c r="M40" s="85"/>
       <c r="O40" s="338" t="s">
-        <v>572</v>
+        <v>605</v>
       </c>
       <c r="P40" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -21087,31 +21200,31 @@
         <v>1</v>
       </c>
       <c r="AA40" t="s">
-        <v>501</v>
+        <v>251</v>
       </c>
       <c r="AB40" t="s">
-        <v>502</v>
+        <v>583</v>
       </c>
       <c r="AC40" s="347" t="s">
-        <v>431</v>
+        <v>514</v>
       </c>
       <c r="AD40" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AE40" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AF40" t="s">
-        <v>503</v>
+        <v>417</v>
       </c>
       <c r="AG40" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="AH40" t="s">
         <v>293</v>
       </c>
       <c r="AJ40" t="s">
-        <v>480</v>
+        <v>384</v>
       </c>
     </row>
     <row r="41" spans="1:36" ht="14.25" x14ac:dyDescent="0.25">
@@ -21143,7 +21256,7 @@
       </c>
       <c r="M41" s="85"/>
       <c r="O41" s="338" t="s">
-        <v>584</v>
+        <v>617</v>
       </c>
       <c r="P41" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -21154,7 +21267,7 @@
         <v>$F$46</v>
       </c>
       <c r="R41" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="S41" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -21170,9 +21283,9 @@
       <c r="V41" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W41" t="e">
+      <c r="W41" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X41" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -21183,31 +21296,31 @@
         <v>1</v>
       </c>
       <c r="AA41" t="s">
-        <v>265</v>
+        <v>536</v>
       </c>
       <c r="AB41" t="s">
-        <v>553</v>
+        <v>584</v>
       </c>
       <c r="AC41" s="347" t="s">
-        <v>514</v>
+        <v>431</v>
       </c>
       <c r="AD41" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AE41" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AF41" t="s">
-        <v>425</v>
+        <v>552</v>
       </c>
       <c r="AG41" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="AH41" t="s">
         <v>293</v>
       </c>
       <c r="AJ41" t="s">
-        <v>384</v>
+        <v>553</v>
       </c>
     </row>
     <row r="42" spans="1:36" x14ac:dyDescent="0.2">
@@ -21219,7 +21332,7 @@
       <c r="E42" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="396" t="s">
+      <c r="F42" s="395" t="s">
         <v>46</v>
       </c>
       <c r="G42" s="214" t="s">
@@ -21239,7 +21352,7 @@
       </c>
       <c r="M42" s="85"/>
       <c r="O42" s="338" t="s">
-        <v>573</v>
+        <v>606</v>
       </c>
       <c r="P42" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -21281,31 +21394,31 @@
         <v>1</v>
       </c>
       <c r="AA42" t="s">
-        <v>504</v>
+        <v>257</v>
       </c>
       <c r="AB42" t="s">
-        <v>339</v>
+        <v>585</v>
       </c>
       <c r="AC42" s="347" t="s">
-        <v>431</v>
+        <v>514</v>
       </c>
       <c r="AD42" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AE42" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="AF42" t="s">
-        <v>505</v>
+        <v>420</v>
       </c>
       <c r="AG42" t="s">
-        <v>351</v>
+        <v>136</v>
       </c>
       <c r="AH42" t="s">
         <v>293</v>
       </c>
       <c r="AJ42" t="s">
-        <v>506</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43" spans="1:36" x14ac:dyDescent="0.2">
@@ -21320,7 +21433,7 @@
       <c r="E43" s="284" t="s">
         <v>40</v>
       </c>
-      <c r="F43" s="396" t="s">
+      <c r="F43" s="395" t="s">
         <v>46</v>
       </c>
       <c r="G43" s="106"/>
@@ -21338,7 +21451,7 @@
       </c>
       <c r="M43" s="85"/>
       <c r="O43" s="338" t="s">
-        <v>574</v>
+        <v>607</v>
       </c>
       <c r="P43" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -21380,28 +21493,34 @@
         <v>1</v>
       </c>
       <c r="AA43" t="s">
-        <v>507</v>
+        <v>259</v>
       </c>
       <c r="AB43" t="s">
-        <v>357</v>
+        <v>586</v>
       </c>
       <c r="AC43" s="347" t="s">
-        <v>469</v>
+        <v>514</v>
       </c>
       <c r="AD43" s="347" t="s">
-        <v>431</v>
+        <v>514</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>191</v>
       </c>
       <c r="AF43" t="s">
-        <v>355</v>
+        <v>421</v>
       </c>
       <c r="AG43" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="AH43" t="s">
-        <v>356</v>
+        <v>293</v>
+      </c>
+      <c r="AI43" t="s">
+        <v>406</v>
       </c>
       <c r="AJ43" t="s">
-        <v>356</v>
+        <v>384</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="14.25" x14ac:dyDescent="0.25">
@@ -21433,7 +21552,7 @@
       </c>
       <c r="M44" s="85"/>
       <c r="O44" s="338" t="s">
-        <v>585</v>
+        <v>618</v>
       </c>
       <c r="P44" s="339">
         <f t="shared" ca="1" si="0"/>
@@ -21444,7 +21563,7 @@
         <v>$B$49</v>
       </c>
       <c r="R44" t="s">
-        <v>537</v>
+        <v>556</v>
       </c>
       <c r="S44" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -21460,9 +21579,9 @@
       <c r="V44" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W44" t="e">
+      <c r="W44" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X44" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -21473,28 +21592,31 @@
         <v>1</v>
       </c>
       <c r="AA44" t="s">
-        <v>358</v>
+        <v>556</v>
       </c>
       <c r="AB44" t="s">
-        <v>360</v>
+        <v>587</v>
       </c>
       <c r="AC44" s="347" t="s">
-        <v>469</v>
+        <v>431</v>
       </c>
       <c r="AD44" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>194</v>
       </c>
       <c r="AF44" t="s">
-        <v>359</v>
+        <v>624</v>
       </c>
       <c r="AG44" t="s">
-        <v>359</v>
+        <v>136</v>
       </c>
       <c r="AH44" t="s">
-        <v>356</v>
+        <v>293</v>
       </c>
       <c r="AJ44" t="s">
-        <v>356</v>
+        <v>554</v>
       </c>
     </row>
     <row r="45" spans="1:36" x14ac:dyDescent="0.2">
@@ -21524,7 +21646,7 @@
       </c>
       <c r="M45" s="85"/>
       <c r="O45" s="338" t="s">
-        <v>586</v>
+        <v>619</v>
       </c>
       <c r="P45" s="339">
         <f t="shared" ca="1" si="0"/>
@@ -21535,7 +21657,7 @@
         <v>$C$49</v>
       </c>
       <c r="R45" t="s">
-        <v>538</v>
+        <v>557</v>
       </c>
       <c r="S45" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -21551,9 +21673,9 @@
       <c r="V45" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W45" t="e">
+      <c r="W45" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X45" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -21564,28 +21686,31 @@
         <v>1</v>
       </c>
       <c r="AA45" t="s">
-        <v>361</v>
+        <v>557</v>
       </c>
       <c r="AB45" t="s">
-        <v>360</v>
+        <v>588</v>
       </c>
       <c r="AC45" s="347" t="s">
-        <v>469</v>
+        <v>431</v>
       </c>
       <c r="AD45" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>194</v>
       </c>
       <c r="AF45" t="s">
-        <v>362</v>
+        <v>625</v>
       </c>
       <c r="AG45" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="AH45" t="s">
-        <v>356</v>
+        <v>293</v>
       </c>
       <c r="AJ45" t="s">
-        <v>356</v>
+        <v>554</v>
       </c>
     </row>
     <row r="46" spans="1:36" ht="14.25" x14ac:dyDescent="0.25">
@@ -21614,7 +21739,7 @@
       </c>
       <c r="M46" s="85"/>
       <c r="O46" s="338" t="s">
-        <v>575</v>
+        <v>608</v>
       </c>
       <c r="P46" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -21656,22 +21781,31 @@
         <v>1</v>
       </c>
       <c r="AA46" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="AB46" t="s">
-        <v>508</v>
+        <v>589</v>
       </c>
       <c r="AC46" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
       </c>
       <c r="AD46" s="347" t="s">
-        <v>186</v>
+        <v>514</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>191</v>
       </c>
       <c r="AF46" t="s">
-        <v>364</v>
+        <v>425</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>351</v>
       </c>
       <c r="AH46" t="s">
-        <v>284</v>
+        <v>293</v>
+      </c>
+      <c r="AJ46" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="47" spans="1:36" x14ac:dyDescent="0.2">
@@ -21703,7 +21837,7 @@
       </c>
       <c r="M47" s="85"/>
       <c r="O47" s="338" t="s">
-        <v>587</v>
+        <v>620</v>
       </c>
       <c r="P47" s="339" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -21714,7 +21848,7 @@
         <v>$F$51</v>
       </c>
       <c r="R47" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="S47" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -21730,9 +21864,9 @@
       <c r="V47" s="348" t="s">
         <v>194</v>
       </c>
-      <c r="W47" t="e">
+      <c r="W47" t="b">
         <f ca="1">EXACT(config34Gy1F[[#This Row],[Address]],VLOOKUP(config34Gy1F[[#This Row],[Name]],Definitions34Gy1F[],2,FALSE))</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="X47" s="348" t="b">
         <f ca="1">IF(EXACT(config34Gy1F[[#This Row],[Extracted Format]],config34Gy1F[[#This Row],[Expected Format]]),TRUE,IF(EXACT(config34Gy1F[[#This Row],[Expected Format]],"@"),"Check",FALSE))</f>
@@ -21743,22 +21877,31 @@
         <v>1</v>
       </c>
       <c r="AA47" t="s">
-        <v>366</v>
+        <v>537</v>
       </c>
       <c r="AB47" t="s">
-        <v>342</v>
+        <v>590</v>
       </c>
       <c r="AC47" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
       </c>
       <c r="AD47" s="347" t="s">
-        <v>186</v>
+        <v>431</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>194</v>
       </c>
       <c r="AF47" t="s">
-        <v>279</v>
+        <v>626</v>
+      </c>
+      <c r="AG47" t="s">
+        <v>351</v>
       </c>
       <c r="AH47" t="s">
-        <v>284</v>
+        <v>293</v>
+      </c>
+      <c r="AJ47" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="48" spans="1:36" x14ac:dyDescent="0.2">
@@ -21789,28 +21932,10 @@
       <c r="M48" s="85"/>
       <c r="O48"/>
       <c r="P48"/>
-      <c r="AA48" t="s">
-        <v>368</v>
-      </c>
-      <c r="AB48" t="s">
-        <v>509</v>
-      </c>
-      <c r="AC48" s="347" t="s">
-        <v>186</v>
-      </c>
-      <c r="AD48" s="347" t="s">
-        <v>186</v>
-      </c>
-      <c r="AF48" t="s">
-        <v>280</v>
-      </c>
-      <c r="AH48" t="s">
-        <v>284</v>
-      </c>
     </row>
     <row r="49" spans="2:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="B49" s="398"/>
-      <c r="C49" s="399"/>
+      <c r="B49" s="397"/>
+      <c r="C49" s="398"/>
       <c r="D49" s="92"/>
       <c r="E49" s="298" t="s">
         <v>168</v>
@@ -21845,7 +21970,7 @@
       <c r="E50" s="289" t="s">
         <v>40</v>
       </c>
-      <c r="F50" s="397" t="s">
+      <c r="F50" s="396" t="s">
         <v>46</v>
       </c>
       <c r="G50" s="15"/>
@@ -21910,177 +22035,177 @@
     <mergeCell ref="D29:E29"/>
   </mergeCells>
   <conditionalFormatting sqref="K14:K15 K46 K19:K27 K41">
-    <cfRule type="containsText" dxfId="46" priority="49" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="40" priority="49" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="containsText" dxfId="45" priority="43" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="39" priority="43" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43">
-    <cfRule type="containsText" dxfId="44" priority="42" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="38" priority="42" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="containsText" dxfId="43" priority="46" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="37" priority="46" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37">
-    <cfRule type="containsText" dxfId="42" priority="45" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="36" priority="45" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38">
-    <cfRule type="containsText" dxfId="41" priority="44" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="35" priority="44" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45">
-    <cfRule type="containsText" dxfId="40" priority="41" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="34" priority="41" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="containsText" dxfId="39" priority="37" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="33" priority="37" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="38" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="32" priority="38" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="39" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="31" priority="39" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="containsText" dxfId="36" priority="31" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="30" priority="31" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="32" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="29" priority="32" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="33" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="28" priority="33" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="33" priority="28" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="27" priority="28" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="29" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="26" priority="29" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="30" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="25" priority="30" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28">
-    <cfRule type="containsText" dxfId="30" priority="24" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="24" priority="24" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="25" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="23" priority="25" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K28)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="26" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="22" priority="26" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29">
-    <cfRule type="containsText" dxfId="27" priority="21" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="21" priority="21" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="22" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="20" priority="22" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K29)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="23" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="19" priority="23" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:K27">
-    <cfRule type="containsText" dxfId="24" priority="20" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="18" priority="20" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="27" stopIfTrue="1" operator="containsText" text="MAJOR">
+    <cfRule type="containsText" dxfId="17" priority="27" stopIfTrue="1" operator="containsText" text="MAJOR">
       <formula>NOT(ISERROR(SEARCH("MAJOR",K20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39">
-    <cfRule type="containsText" dxfId="22" priority="18" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="16" priority="18" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40">
-    <cfRule type="containsText" dxfId="21" priority="17" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="15" priority="17" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="containsText" dxfId="20" priority="16" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="14" priority="16" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35">
-    <cfRule type="containsText" dxfId="19" priority="15" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="13" priority="15" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36">
-    <cfRule type="containsText" dxfId="18" priority="14" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="12" priority="14" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="containsText" dxfId="17" priority="12" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="11" priority="12" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32">
-    <cfRule type="containsText" dxfId="16" priority="11" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="10" priority="11" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="containsText" dxfId="15" priority="10" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="9" priority="10" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33">
-    <cfRule type="containsText" dxfId="14" priority="9" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="8" priority="9" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50:K51">
-    <cfRule type="containsText" dxfId="13" priority="8" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="7" priority="8" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:K49">
-    <cfRule type="containsText" dxfId="12" priority="7" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="6" priority="7" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="11" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
+    <cfRule type="containsText" dxfId="5" priority="4" stopIfTrue="1" operator="containsText" text="Minor">
       <formula>NOT(ISERROR(SEARCH("Minor",K18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" stopIfTrue="1" operator="containsText" text="No">
+    <cfRule type="containsText" dxfId="4" priority="5" stopIfTrue="1" operator="containsText" text="No">
       <formula>NOT(ISERROR(SEARCH("No",K18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" stopIfTrue="1" operator="containsText" text="Major">
+    <cfRule type="containsText" dxfId="3" priority="6" stopIfTrue="1" operator="containsText" text="Major">
       <formula>NOT(ISERROR(SEARCH("Major",K18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W4:Y47">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>W4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>EXACT(W4,"Check")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>W4=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>